<commit_message>
Pruebas Funcionales - No Funcionales
Se completa las pruebas NO Funcionales
</commit_message>
<xml_diff>
--- a/Documentación/Pruebas/Descripcion Responsabilidades pruebas.xlsx
+++ b/Documentación/Pruebas/Descripcion Responsabilidades pruebas.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17927"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Pol_Ing_Sis\8-Ingenieria de Software 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\precise_estimate\Documentación\Pruebas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -250,7 +250,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -548,11 +548,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="14.25" customWidth="1"/>
     <col min="2" max="2" width="18.125" customWidth="1"/>
@@ -588,42 +588,42 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" ht="28.5">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" ht="28.5">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" ht="28.5">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" ht="28.5">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" ht="28.5">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" ht="28.5">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="2" t="s">
@@ -669,7 +669,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" ht="28.5">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="2" t="s">
@@ -690,14 +690,14 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" ht="28.5">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" ht="28.5">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="2" t="s">
@@ -722,21 +722,21 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" ht="28.5">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" ht="28.5">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="28.5">
+    <row r="24" spans="1:3" ht="42.75">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="2" t="s">
@@ -750,7 +750,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" ht="28.5">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="2" t="s">
@@ -775,7 +775,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" ht="28.5">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="2" t="s">
@@ -796,7 +796,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" ht="28.5">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="2" t="s">

</xml_diff>